<commit_message>
new changes in the architecture
</commit_message>
<xml_diff>
--- a/Boards/PIC18F4550/ControlePID/documentation/Especificação Técnica.xlsx
+++ b/Boards/PIC18F4550/ControlePID/documentation/Especificação Técnica.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="474" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="-180" windowWidth="17430" windowHeight="8565" tabRatio="474" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos_Firmware" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">Requsitos_Hardware!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="151">
   <si>
     <t>Projeto:  Template</t>
   </si>
@@ -521,6 +521,15 @@
   <si>
     <t>Sensor de temperatura</t>
   </si>
+  <si>
+    <t>JAGA PIN</t>
+  </si>
+  <si>
+    <t>Projeto:</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
 </sst>
 </file>
 
@@ -529,7 +538,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -602,8 +611,22 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -706,8 +729,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -754,11 +783,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -893,17 +933,26 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1279,20 +1328,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
@@ -1343,44 +1392,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:K48"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17"/>
-    <col min="2" max="2" width="31.5703125"/>
-    <col min="3" max="3" width="8.85546875"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125"/>
-    <col min="7" max="7" width="16.140625"/>
-    <col min="8" max="8" width="13.140625"/>
-    <col min="9" max="9" width="10.5703125"/>
-    <col min="10" max="10" width="44"/>
-    <col min="11" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17"/>
+    <col min="3" max="3" width="31.5703125"/>
+    <col min="4" max="4" width="8.85546875"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125"/>
+    <col min="8" max="8" width="16.140625"/>
+    <col min="9" max="9" width="13.140625"/>
+    <col min="10" max="10" width="10.5703125"/>
+    <col min="11" max="11" width="44"/>
+    <col min="12" max="1026" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="1" spans="1:12">
+      <c r="A1" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1388,7 +1446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1396,7 +1454,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1404,884 +1462,1007 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="18.75">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:12" ht="18.75">
+      <c r="A8" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="K8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="L8" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="10">
+    <row r="9" spans="1:12" ht="15.75">
+      <c r="A9" s="66">
+        <v>0</v>
+      </c>
+      <c r="B9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="I9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="J9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="K9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="64">
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75">
+      <c r="A10" s="66">
+        <v>1</v>
+      </c>
+      <c r="B10" s="63">
         <v>2</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="C10" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="D10" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="E10" s="63" t="s">
         <v>146</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="F10" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="H10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="K10" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="22"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="17">
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75">
+      <c r="A11" s="66">
+        <v>2</v>
+      </c>
+      <c r="B11" s="17">
         <v>3</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C11" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="61"/>
       <c r="D11" s="61"/>
-      <c r="E11" s="30"/>
-      <c r="G11" s="19" t="s">
+      <c r="E11" s="61"/>
+      <c r="F11" s="30"/>
+      <c r="H11" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="20"/>
+      <c r="J11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="K11" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="22"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="17">
+      <c r="L11" s="22"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75">
+      <c r="A12" s="66">
+        <v>3</v>
+      </c>
+      <c r="B12" s="17">
         <v>4</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="61"/>
       <c r="D12" s="61"/>
-      <c r="E12" s="30"/>
-      <c r="G12" s="19" t="s">
+      <c r="E12" s="61"/>
+      <c r="F12" s="30"/>
+      <c r="H12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="20"/>
+      <c r="J12" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="K12" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="22"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="17">
+      <c r="L12" s="22"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75">
+      <c r="A13" s="66">
+        <v>4</v>
+      </c>
+      <c r="B13" s="17">
         <v>5</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="C13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="61"/>
       <c r="D13" s="61"/>
-      <c r="E13" s="30"/>
-      <c r="G13" s="19" t="s">
+      <c r="E13" s="61"/>
+      <c r="F13" s="30"/>
+      <c r="H13" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="22"/>
+      <c r="J13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="K13" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="22"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="23">
+      <c r="L13" s="22"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75">
+      <c r="A14" s="66">
+        <v>5</v>
+      </c>
+      <c r="B14" s="23">
         <v>6</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="C14" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="D14" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="E14" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="G14" s="19" t="s">
+      <c r="F14" s="17"/>
+      <c r="H14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="22"/>
+      <c r="J14" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="K14" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="22"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="23">
+      <c r="L14" s="22"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
+      <c r="A15" s="66">
+        <v>6</v>
+      </c>
+      <c r="B15" s="23">
         <v>7</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="C15" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="D15" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="E15" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="G15" s="19" t="s">
+      <c r="F15" s="1"/>
+      <c r="H15" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="22"/>
+      <c r="J15" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="21" t="s">
+      <c r="K15" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="22"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="17">
+      <c r="L15" s="22"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75">
+      <c r="A16" s="66">
+        <v>7</v>
+      </c>
+      <c r="B16" s="17">
         <v>8</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="C16" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="17"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="17"/>
-      <c r="G16" s="19" t="s">
+      <c r="F16" s="17"/>
+      <c r="H16" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="22"/>
+      <c r="J16" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="K16" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="K16" s="22"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="27">
+      <c r="L16" s="22"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
+      <c r="A17" s="66">
+        <v>8</v>
+      </c>
+      <c r="B17" s="27">
         <v>9</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="C17" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="D17" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="E17" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="G17" s="19" t="s">
+      <c r="F17" s="30"/>
+      <c r="H17" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="22"/>
+      <c r="J17" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="21" t="s">
+      <c r="K17" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="K17" s="22"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="27">
+      <c r="L17" s="22"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75">
+      <c r="A18" s="66">
+        <v>9</v>
+      </c>
+      <c r="B18" s="27">
         <v>10</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="C18" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="D18" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="E18" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="G18" s="19" t="s">
+      <c r="F18" s="17"/>
+      <c r="H18" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="22"/>
+      <c r="J18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="K18" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="22"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="31">
+      <c r="L18" s="22"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
+      <c r="A19" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="31">
         <v>11</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="C19" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="D19" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="E19" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="63" t="s">
+      <c r="F19" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="H19" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="35" t="s">
+      <c r="I19" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="35" t="s">
+      <c r="J19" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="J19" s="36" t="s">
+      <c r="K19" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="K19" s="22"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="37">
+      <c r="L19" s="22"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75">
+      <c r="A20" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="37">
         <v>12</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="C20" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="D20" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="E20" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="63">
+      <c r="F20" s="62">
         <v>0</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="H20" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="22"/>
+      <c r="J20" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="K20" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="22"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="40">
+      <c r="L20" s="22"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75">
+      <c r="A21" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="40">
         <v>13</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="C21" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="D21" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="E21" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="G21" s="19" t="s">
+      <c r="F21" s="62"/>
+      <c r="H21" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="22"/>
+      <c r="J21" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="21" t="s">
+      <c r="K21" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="K21" s="22"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="40">
+      <c r="L21" s="22"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75">
+      <c r="A22" s="66">
+        <v>10</v>
+      </c>
+      <c r="B22" s="40">
         <v>14</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="C22" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="D22" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="E22" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="G22" s="19" t="s">
+      <c r="F22" s="62"/>
+      <c r="H22" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="22"/>
+      <c r="J22" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="21" t="s">
+      <c r="K22" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="K22" s="22"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="17">
+      <c r="L22" s="22"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75">
+      <c r="A23" s="66">
+        <v>11</v>
+      </c>
+      <c r="B23" s="17">
         <v>15</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="C23" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="63"/>
-      <c r="G23" s="19" t="s">
+      <c r="D23" s="26"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="62"/>
+      <c r="H23" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="22"/>
+      <c r="J23" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="21" t="s">
+      <c r="K23" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="K23" s="22"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="17">
+      <c r="L23" s="22"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75">
+      <c r="A24" s="66">
+        <v>12</v>
+      </c>
+      <c r="B24" s="17">
         <v>16</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="C24" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="63"/>
-      <c r="G24" s="19" t="s">
+      <c r="D24" s="26"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="62"/>
+      <c r="H24" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="22"/>
+      <c r="J24" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="21" t="s">
+      <c r="K24" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="K24" s="22"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="44">
+      <c r="L24" s="22"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75">
+      <c r="A25" s="66">
+        <v>13</v>
+      </c>
+      <c r="B25" s="44">
         <v>17</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="C25" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="D25" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="E25" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="G25" s="19" t="s">
+      <c r="F25" s="62"/>
+      <c r="H25" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="22"/>
+      <c r="J25" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="21" t="s">
+      <c r="K25" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="K25" s="22"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="17">
+      <c r="L25" s="22"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75">
+      <c r="A26" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="17">
         <v>18</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="C26" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="63"/>
-      <c r="G26" s="19" t="s">
+      <c r="D26" s="26"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="62"/>
+      <c r="H26" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="20" t="s">
+      <c r="I26" s="22"/>
+      <c r="J26" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="21" t="s">
+      <c r="K26" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="K26" s="22"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="47">
+      <c r="L26" s="22"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75">
+      <c r="A27" s="66">
+        <v>14</v>
+      </c>
+      <c r="B27" s="47">
         <v>19</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="C27" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="D27" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="47" t="s">
+      <c r="E27" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E27" s="63"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="47">
+      <c r="F27" s="62"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75">
+      <c r="A28" s="66">
+        <v>15</v>
+      </c>
+      <c r="B28" s="47">
         <v>20</v>
       </c>
-      <c r="B28" s="48" t="s">
+      <c r="C28" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="D28" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="E28" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="63"/>
-      <c r="G28" s="19" t="s">
+      <c r="F28" s="62"/>
+      <c r="H28" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="20" t="s">
+      <c r="I28" s="22"/>
+      <c r="J28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="21" t="s">
+      <c r="K28" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="K28" s="22"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="50">
+      <c r="L28" s="22"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75">
+      <c r="A29" s="66">
+        <v>16</v>
+      </c>
+      <c r="B29" s="50">
         <v>21</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="C29" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="52" t="s">
+      <c r="D29" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="50" t="s">
+      <c r="E29" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="E29" s="63" t="s">
+      <c r="F29" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="H29" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="20" t="s">
+      <c r="I29" s="22"/>
+      <c r="J29" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="21" t="s">
+      <c r="K29" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="K29" s="22"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="50">
+      <c r="L29" s="22"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75">
+      <c r="A30" s="66">
+        <v>17</v>
+      </c>
+      <c r="B30" s="50">
         <v>22</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="C30" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="D30" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="50" t="s">
+      <c r="E30" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="63" t="s">
+      <c r="F30" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="H30" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="20" t="s">
+      <c r="I30" s="22"/>
+      <c r="J30" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="53" t="s">
+      <c r="K30" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="K30" s="22"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="17">
+      <c r="L30" s="22"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75">
+      <c r="A31" s="66">
+        <v>18</v>
+      </c>
+      <c r="B31" s="17">
         <v>23</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="C31" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="63"/>
-      <c r="G31" s="19" t="s">
+      <c r="D31" s="26"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="62"/>
+      <c r="H31" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="20" t="s">
+      <c r="I31" s="22"/>
+      <c r="J31" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="21" t="s">
+      <c r="K31" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="K31" s="22"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="17">
+      <c r="L31" s="22"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75">
+      <c r="A32" s="66">
+        <v>19</v>
+      </c>
+      <c r="B32" s="17">
         <v>24</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="C32" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="63"/>
-      <c r="G32" s="19" t="s">
+      <c r="D32" s="26"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="62"/>
+      <c r="H32" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="H32" s="22"/>
-      <c r="I32" s="20" t="s">
+      <c r="I32" s="22"/>
+      <c r="J32" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="21" t="s">
+      <c r="K32" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="K32" s="22"/>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="54">
+      <c r="L32" s="22"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75">
+      <c r="A33" s="66">
+        <v>20</v>
+      </c>
+      <c r="B33" s="54">
         <v>25</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="C33" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="D33" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="54" t="s">
+      <c r="E33" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="G33" s="19" t="s">
+      <c r="F33" s="62"/>
+      <c r="H33" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="20" t="s">
+      <c r="I33" s="22"/>
+      <c r="J33" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J33" s="21" t="s">
+      <c r="K33" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="K33" s="22"/>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="54">
+      <c r="L33" s="22"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75">
+      <c r="A34" s="66">
+        <v>21</v>
+      </c>
+      <c r="B34" s="54">
         <v>26</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="C34" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="D34" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="54" t="s">
+      <c r="E34" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="E34" s="63"/>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="47">
+      <c r="F34" s="62"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75">
+      <c r="A35" s="66">
+        <v>22</v>
+      </c>
+      <c r="B35" s="47">
         <v>27</v>
       </c>
-      <c r="B35" s="48" t="s">
+      <c r="C35" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="D35" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="E35" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="E35" s="63"/>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="47">
+      <c r="F35" s="62"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.75">
+      <c r="A36" s="66">
+        <v>23</v>
+      </c>
+      <c r="B36" s="47">
         <v>28</v>
       </c>
-      <c r="B36" s="48" t="s">
+      <c r="C36" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="D36" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="E36" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="E36" s="63"/>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="47">
+      <c r="F36" s="62"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75">
+      <c r="A37" s="66">
+        <v>24</v>
+      </c>
+      <c r="B37" s="47">
         <v>29</v>
       </c>
-      <c r="B37" s="48" t="s">
+      <c r="C37" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="D37" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="47" t="s">
+      <c r="E37" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="E37" s="63"/>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="47">
+      <c r="F37" s="62"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75">
+      <c r="A38" s="66">
+        <v>25</v>
+      </c>
+      <c r="B38" s="47">
         <v>30</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="C38" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="D38" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="47" t="s">
+      <c r="E38" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="E38" s="63"/>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="31">
+      <c r="F38" s="62"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75">
+      <c r="A39" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="31">
         <v>31</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="C39" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="D39" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="E39" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="63" t="s">
+      <c r="F39" s="62" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="37">
+    <row r="40" spans="1:12" ht="15.75">
+      <c r="A40" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="37">
         <v>32</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="C40" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="D40" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="37" t="s">
+      <c r="E40" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E40" s="63">
+      <c r="F40" s="62">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="57">
+    <row r="41" spans="1:12" ht="15.75">
+      <c r="A41" s="67">
+        <v>26</v>
+      </c>
+      <c r="B41" s="57">
         <v>33</v>
       </c>
-      <c r="B41" s="58" t="s">
+      <c r="C41" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57" t="s">
+      <c r="D41" s="57"/>
+      <c r="E41" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="F41" s="30" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="57">
+    <row r="42" spans="1:12" ht="15.75">
+      <c r="A42" s="66">
+        <v>27</v>
+      </c>
+      <c r="B42" s="57">
         <v>34</v>
       </c>
-      <c r="B42" s="58" t="s">
+      <c r="C42" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57" t="s">
+      <c r="D42" s="57"/>
+      <c r="E42" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="F42" s="17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="27">
+    <row r="43" spans="1:12" ht="15.75">
+      <c r="A43" s="66">
+        <v>28</v>
+      </c>
+      <c r="B43" s="27">
         <v>35</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="C43" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="D43" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="27" t="s">
+      <c r="E43" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="30"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="27">
+      <c r="F43" s="30"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75">
+      <c r="A44" s="66">
+        <v>29</v>
+      </c>
+      <c r="B44" s="27">
         <v>36</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="C44" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="D44" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="27" t="s">
+      <c r="E44" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="E44" s="17"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="17">
+      <c r="F44" s="17"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75">
+      <c r="A45" s="66">
+        <v>30</v>
+      </c>
+      <c r="B45" s="17">
         <v>37</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="C45" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="17"/>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="59">
+      <c r="F45" s="17"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75">
+      <c r="A46" s="66">
+        <v>31</v>
+      </c>
+      <c r="B46" s="59">
         <v>38</v>
       </c>
-      <c r="B46" s="60" t="s">
+      <c r="C46" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="59" t="s">
+      <c r="D46" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="D46" s="59" t="s">
+      <c r="E46" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="E46" s="63"/>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="59">
+      <c r="F46" s="62"/>
+    </row>
+    <row r="47" spans="1:12" ht="15.75">
+      <c r="A47" s="66">
+        <v>32</v>
+      </c>
+      <c r="B47" s="59">
         <v>39</v>
       </c>
-      <c r="B47" s="60" t="s">
+      <c r="C47" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="59" t="s">
+      <c r="D47" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="D47" s="59" t="s">
+      <c r="E47" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="E47" s="63"/>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="59">
+      <c r="F47" s="62"/>
+    </row>
+    <row r="48" spans="1:12" ht="15.75">
+      <c r="A48" s="66">
+        <v>33</v>
+      </c>
+      <c r="B48" s="59">
         <v>40</v>
       </c>
-      <c r="B48" s="60" t="s">
+      <c r="C48" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="59" t="s">
+      <c r="D48" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="D48" s="59" t="s">
+      <c r="E48" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="E48" s="63"/>
+      <c r="F48" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>